<commit_message>
Dependencies: Upgrade Charset Normalizer to 2.0.6
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3BA931-2277-49F8-AE57-B6454C9F0D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA26584-A8F3-4615-A9FD-DF11A8195721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,9 +490,6 @@
     <t>https://github.com/Ousret/charset_normalizer</t>
   </si>
   <si>
-    <t>2.0.4</t>
-  </si>
-  <si>
     <t>TAHRI Ahmed R.</t>
   </si>
   <si>
@@ -650,6 +647,9 @@
   <si>
     <t>Matthew Honnibal, Ines Montani, Sofie Van Landeghem,
 Adriane Boyd, Paul O'Leary McCann</t>
+  </si>
+  <si>
+    <t>2.0.6</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1115,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1227,7 +1227,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>18</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>37</v>
@@ -1327,7 +1327,7 @@
         <v>58</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>18</v>
@@ -1387,7 +1387,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>31</v>
@@ -1447,7 +1447,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>18</v>
@@ -1501,7 +1501,7 @@
         <v>98</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>99</v>
@@ -1805,7 +1805,7 @@
         <v>135</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>143</v>
@@ -1825,7 +1825,7 @@
         <v>139</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>144</v>
@@ -1862,7 +1862,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1924,176 +1924,176 @@
         <v>152</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>137</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>137</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>193</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>194</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>137</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependencies: Upgrade spaCy to 3.1.3
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BC96C3-B6FC-41AA-9583-4447787E9C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9101F0F8-585A-4FA4-B3B7-76186663842E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,9 +261,6 @@
     <t>spaCy</t>
   </si>
   <si>
-    <t>3.1.1</t>
-  </si>
-  <si>
     <t>https://github.com/explosion/spaCy/blob/master/LICENSE</t>
   </si>
   <si>
@@ -631,6 +628,9 @@
   </si>
   <si>
     <t>1.7.1</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1005,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,22 +1041,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>138</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1081,22 +1081,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1110,7 +1110,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
@@ -1121,27 +1121,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>32</v>
@@ -1161,122 +1161,122 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1301,22 +1301,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1327,7 +1327,7 @@
         <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>43</v>
@@ -1341,22 +1341,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1381,22 +1381,22 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="C19" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1410,7 +1410,7 @@
         <v>52</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>14</v>
@@ -1496,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1507,10 +1507,10 @@
         <v>66</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>26</v>
@@ -1541,22 +1541,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,22 +1581,22 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1607,7 +1607,7 @@
         <v>74</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>75</v>
@@ -1621,22 +1621,22 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1644,159 +1644,159 @@
         <v>77</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>78</v>
+        <v>200</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependencies: Upgrade Tokenizer to 3.3.2
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9101F0F8-585A-4FA4-B3B7-76186663842E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661F8E11-7F6D-436D-8E57-6FB0D3CF3F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,9 +312,6 @@
     <t>https://github.com/mideind/Tokenizer</t>
   </si>
   <si>
-    <t>3.1.2</t>
-  </si>
-  <si>
     <t>Vilhjálmur Þorsteinsson</t>
   </si>
   <si>
@@ -631,6 +628,9 @@
   </si>
   <si>
     <t>3.1.3</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1005,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,22 +1041,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1081,22 +1081,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1110,7 +1110,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
@@ -1121,27 +1121,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>32</v>
@@ -1161,122 +1161,122 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1301,22 +1301,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1327,7 +1327,7 @@
         <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>43</v>
@@ -1341,22 +1341,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1381,22 +1381,22 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="C19" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1410,7 +1410,7 @@
         <v>52</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>14</v>
@@ -1496,7 +1496,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1507,10 +1507,10 @@
         <v>66</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>26</v>
@@ -1541,22 +1541,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,22 +1581,22 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1607,7 +1607,7 @@
         <v>74</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>75</v>
@@ -1621,22 +1621,22 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1644,13 +1644,13 @@
         <v>77</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>14</v>
@@ -1681,22 +1681,22 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1724,7 +1724,7 @@
         <v>89</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>90</v>
@@ -1747,56 +1747,56 @@
         <v>94</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependencies: Upgrade PyInstaller to 4.5.1
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661F8E11-7F6D-436D-8E57-6FB0D3CF3F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F231FA33-B19C-4A98-B3D7-6F0A6647A8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="202">
   <si>
     <t>Python</t>
   </si>
@@ -631,6 +631,9 @@
   </si>
   <si>
     <t>3.3.2</t>
+  </si>
+  <si>
+    <t>4.5.1</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1008,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1426,8 +1429,8 @@
       <c r="B21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="6">
-        <v>4.4000000000000004</v>
+      <c r="C21" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Dependencies: Upgrade botok to 0.8.8; Utils: Update botok's Tibetan sentence tokenizer
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F231FA33-B19C-4A98-B3D7-6F0A6647A8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD73191-7578-4213-89D8-B6ED57C6889B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>https://github.com/Esukhia/botok</t>
   </si>
   <si>
-    <t>0.8.7</t>
-  </si>
-  <si>
     <t>Hélios Drupchen Hildt</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>4.5.1</t>
+  </si>
+  <si>
+    <t>0.8.8</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1005,10 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,22 +1044,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1070,356 +1070,356 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="C19" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1430,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
@@ -1444,42 +1444,42 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1499,27 +1499,27 @@
         <v>13</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1544,262 +1544,262 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="C37" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependencies: Upgrade Charset Normalizer to 2.0.7
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD73191-7578-4213-89D8-B6ED57C6889B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B15E6A-94AA-43C8-A297-5D4475FDA9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,9 +594,6 @@
 Adriane Boyd, Paul O'Leary McCann</t>
   </si>
   <si>
-    <t>2.0.6</t>
-  </si>
-  <si>
     <t>4.10.0</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>0.8.8</t>
+  </si>
+  <si>
+    <t>2.0.7</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1008,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,7 +1050,7 @@
         <v>134</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>135</v>
@@ -1070,7 +1070,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
@@ -1090,7 +1090,7 @@
         <v>138</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>139</v>
@@ -1270,7 +1270,7 @@
         <v>121</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>122</v>
@@ -1310,7 +1310,7 @@
         <v>179</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>125</v>
@@ -1330,7 +1330,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>42</v>
@@ -1350,7 +1350,7 @@
         <v>158</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>159</v>
@@ -1390,7 +1390,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>163</v>
@@ -1430,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
@@ -1510,7 +1510,7 @@
         <v>65</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>184</v>
@@ -1610,7 +1610,7 @@
         <v>73</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>74</v>
@@ -1630,7 +1630,7 @@
         <v>175</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>176</v>
@@ -1650,7 +1650,7 @@
         <v>132</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>187</v>
@@ -1750,7 +1750,7 @@
         <v>93</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Dependencies: Upgrade NLTK to 3.6.5
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B15E6A-94AA-43C8-A297-5D4475FDA9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15636F2C-C0F2-4A48-8CA0-FE32D39360FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -603,9 +603,6 @@
     <t>2.6.3</t>
   </si>
   <si>
-    <t>3.6.4</t>
-  </si>
-  <si>
     <t>1.21.2</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>2.0.7</t>
+  </si>
+  <si>
+    <t>3.6.5</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1005,10 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,7 +1070,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
@@ -1090,7 +1090,7 @@
         <v>138</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>139</v>
@@ -1330,7 +1330,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>42</v>
@@ -1350,7 +1350,7 @@
         <v>158</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>159</v>
@@ -1390,7 +1390,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>163</v>
@@ -1430,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
@@ -1510,7 +1510,7 @@
         <v>65</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>184</v>
@@ -1610,7 +1610,7 @@
         <v>73</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>74</v>
@@ -1630,7 +1630,7 @@
         <v>175</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>176</v>
@@ -1650,7 +1650,7 @@
         <v>132</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>187</v>
@@ -1750,7 +1750,7 @@
         <v>93</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Dependencies: Upgrade Charset Normalizer to 2.0.9
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15636F2C-C0F2-4A48-8CA0-FE32D39360FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF263D3-5483-4F01-919D-1CDCF2D287DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,10 +630,10 @@
     <t>0.8.8</t>
   </si>
   <si>
-    <t>2.0.7</t>
-  </si>
-  <si>
     <t>3.6.5</t>
+  </si>
+  <si>
+    <t>2.0.9</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1005,10 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,7 +1090,7 @@
         <v>138</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>139</v>
@@ -1330,7 +1330,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Dependencies: Upgrade spaCy to 3.2.1
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF263D3-5483-4F01-919D-1CDCF2D287DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A950B16C-E811-4AEF-9810-353DBC1BD1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,9 +618,6 @@
     <t>1.7.1</t>
   </si>
   <si>
-    <t>3.1.3</t>
-  </si>
-  <si>
     <t>3.3.2</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>2.0.9</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1005,10 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,7 +1070,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
@@ -1090,7 +1090,7 @@
         <v>138</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>139</v>
@@ -1330,7 +1330,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>42</v>
@@ -1430,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
@@ -1650,7 +1650,7 @@
         <v>132</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>187</v>
@@ -1750,7 +1750,7 @@
         <v>93</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Dependencies: Remove lemmalist-greek; Utils: Remove lemmalist-greek's Greek (Ancient) lemma list
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A950B16C-E811-4AEF-9810-353DBC1BD1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1453F006-BD31-48FE-A839-B3F7266E3CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="198">
   <si>
     <t>Python</t>
   </si>
@@ -343,18 +343,6 @@
   </si>
   <si>
     <t>https://github.com/Xangis/extra-stopwords/blob/master/LICENSE</t>
-  </si>
-  <si>
-    <t>lemmalist-greek</t>
-  </si>
-  <si>
-    <t>https://github.com/stenskjaer/lemmalist-greek</t>
-  </si>
-  <si>
-    <t>Michael Stenskjær Christensen</t>
-  </si>
-  <si>
-    <t>https://github.com/stenskjaer/lemmalist-greek/blob/master/LICENSE</t>
   </si>
   <si>
     <t>Lemmatization Lists</t>
@@ -1002,13 +990,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C140BD20-F5FB-434E-99AB-C043EB24C86B}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,22 +1032,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1070,7 +1058,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
@@ -1084,22 +1072,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1113,7 +1101,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
@@ -1144,7 +1132,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -1164,42 +1152,42 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="F9" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1216,676 +1204,654 @@
         <v>108</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>122</v>
+        <v>38</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>37</v>
+        <v>186</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>124</v>
+        <v>40</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>179</v>
+        <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>158</v>
+        <v>45</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>191</v>
+        <v>46</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>160</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>46</v>
+        <v>188</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>161</v>
+        <v>49</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>162</v>
+        <v>50</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>163</v>
+        <v>51</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="E20" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>8</v>
+      <c r="F21" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E22" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>21</v>
+      <c r="F26" s="8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>165</v>
+        <v>67</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>167</v>
+        <v>69</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>168</v>
+        <v>70</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>170</v>
+        <v>72</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>178</v>
+        <v>73</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>172</v>
+        <v>74</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>173</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>72</v>
+        <v>170</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="E30" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>126</v>
-      </c>
       <c r="F31" s="8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>187</v>
+        <v>80</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>84</v>
+        <v>177</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>89</v>
+        <v>192</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>196</v>
+        <v>98</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
-    <sortCondition ref="A2:A39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F38">
+    <sortCondition ref="A2:A38"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CF73D8A8-B4D6-4683-89DA-FFC51092EBEB}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{771C650C-0717-49FD-B0EC-BF2F40F224EB}"/>
     <hyperlink ref="B8" r:id="rId3" xr:uid="{E12C1CA8-5B68-4852-BA02-BD7BBD2E879E}"/>
     <hyperlink ref="B9" r:id="rId4" xr:uid="{1663737B-16F3-42B6-90CA-BFEB7DCE1174}"/>
-    <hyperlink ref="B12" r:id="rId5" xr:uid="{13EDF357-B8BF-4BDF-8117-199BDDBEB4EF}"/>
-    <hyperlink ref="B17" r:id="rId6" xr:uid="{A0E84A41-E233-42F2-BD8A-A1BDF1E81869}"/>
-    <hyperlink ref="B19" r:id="rId7" xr:uid="{4F5A65A0-DA16-4EAA-8204-89C4587728EC}"/>
-    <hyperlink ref="B27" r:id="rId8" xr:uid="{D806A658-6D50-416A-8F31-9519F420DB6F}"/>
-    <hyperlink ref="B29" r:id="rId9" xr:uid="{AE9E7534-DCC6-43F9-9F7E-CB7D0988653C}"/>
-    <hyperlink ref="B31" r:id="rId10" xr:uid="{48E985F1-8312-44D5-B359-BC5428959610}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{13EDF357-B8BF-4BDF-8117-199BDDBEB4EF}"/>
+    <hyperlink ref="B16" r:id="rId6" xr:uid="{A0E84A41-E233-42F2-BD8A-A1BDF1E81869}"/>
+    <hyperlink ref="B18" r:id="rId7" xr:uid="{4F5A65A0-DA16-4EAA-8204-89C4587728EC}"/>
+    <hyperlink ref="B26" r:id="rId8" xr:uid="{D806A658-6D50-416A-8F31-9519F420DB6F}"/>
+    <hyperlink ref="B28" r:id="rId9" xr:uid="{AE9E7534-DCC6-43F9-9F7E-CB7D0988653C}"/>
+    <hyperlink ref="B30" r:id="rId10" xr:uid="{48E985F1-8312-44D5-B359-BC5428959610}"/>
     <hyperlink ref="F2" r:id="rId11" xr:uid="{929E88FE-A5CA-4C8A-AB63-CC5216646638}"/>
     <hyperlink ref="F4" r:id="rId12" xr:uid="{FF1D0CA5-516F-4B32-914F-109BD9394062}"/>
     <hyperlink ref="F8" r:id="rId13" xr:uid="{56571F8E-94F9-4E59-8301-FD9B586601E2}"/>
     <hyperlink ref="F9" r:id="rId14" xr:uid="{4E203B3A-56CE-4F2E-8E50-ECD13E173A62}"/>
-    <hyperlink ref="F12" r:id="rId15" xr:uid="{F43F53F1-7279-4683-9981-2134AA1FD339}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{C85E458B-00C2-411B-B49E-AE8022969698}"/>
-    <hyperlink ref="F19" r:id="rId17" xr:uid="{976B8A16-77B7-4FEF-9169-6BBFE075FCA3}"/>
-    <hyperlink ref="F27" r:id="rId18" xr:uid="{A52538D1-12B7-46FF-8221-0E6B9ABCA510}"/>
-    <hyperlink ref="F29" r:id="rId19" xr:uid="{7E1954E6-38DA-415E-A3C7-E1A13CC34AA6}"/>
-    <hyperlink ref="F31" r:id="rId20" xr:uid="{24AF1213-EF9C-4A65-A07F-FA87ED52B38E}"/>
-    <hyperlink ref="F26" r:id="rId21" location="psf-license-agreement-for-python-release" xr:uid="{F5F51C21-2025-43C8-A97E-01655AD44B0D}"/>
-    <hyperlink ref="F21" r:id="rId22" xr:uid="{5E4BF004-2691-47C7-8862-14F66FADDDD6}"/>
-    <hyperlink ref="F24" r:id="rId23" location="license" xr:uid="{660E8A5C-2DFD-41A4-861A-90E9BF510D8D}"/>
-    <hyperlink ref="B26" r:id="rId24" xr:uid="{D099E31D-9265-415C-969C-6D26EB302243}"/>
-    <hyperlink ref="B21" r:id="rId25" xr:uid="{5AE99205-01DB-477E-A6BD-69F46164974B}"/>
-    <hyperlink ref="B24" r:id="rId26" xr:uid="{0F7B6A32-4F56-4F52-A479-8662313527D4}"/>
-    <hyperlink ref="B13" r:id="rId27" xr:uid="{2C8B3443-48AE-472B-8B71-94EE65EDAD01}"/>
-    <hyperlink ref="B15" r:id="rId28" xr:uid="{304D21BB-CA92-4A54-8547-375084292F85}"/>
-    <hyperlink ref="F13" r:id="rId29" xr:uid="{9008EE1B-E8AE-4A0D-984F-B12DD1DAB45D}"/>
-    <hyperlink ref="F15" r:id="rId30" xr:uid="{573D0817-1969-4B68-A9EA-1A1C9EFBCC06}"/>
-    <hyperlink ref="B39" r:id="rId31" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
-    <hyperlink ref="F39" r:id="rId32" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
+    <hyperlink ref="F11" r:id="rId15" xr:uid="{F43F53F1-7279-4683-9981-2134AA1FD339}"/>
+    <hyperlink ref="F16" r:id="rId16" xr:uid="{C85E458B-00C2-411B-B49E-AE8022969698}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{976B8A16-77B7-4FEF-9169-6BBFE075FCA3}"/>
+    <hyperlink ref="F26" r:id="rId18" xr:uid="{A52538D1-12B7-46FF-8221-0E6B9ABCA510}"/>
+    <hyperlink ref="F28" r:id="rId19" xr:uid="{7E1954E6-38DA-415E-A3C7-E1A13CC34AA6}"/>
+    <hyperlink ref="F30" r:id="rId20" xr:uid="{24AF1213-EF9C-4A65-A07F-FA87ED52B38E}"/>
+    <hyperlink ref="F25" r:id="rId21" location="psf-license-agreement-for-python-release" xr:uid="{F5F51C21-2025-43C8-A97E-01655AD44B0D}"/>
+    <hyperlink ref="F20" r:id="rId22" xr:uid="{5E4BF004-2691-47C7-8862-14F66FADDDD6}"/>
+    <hyperlink ref="F23" r:id="rId23" location="license" xr:uid="{660E8A5C-2DFD-41A4-861A-90E9BF510D8D}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{D099E31D-9265-415C-969C-6D26EB302243}"/>
+    <hyperlink ref="B20" r:id="rId25" xr:uid="{5AE99205-01DB-477E-A6BD-69F46164974B}"/>
+    <hyperlink ref="B23" r:id="rId26" xr:uid="{0F7B6A32-4F56-4F52-A479-8662313527D4}"/>
+    <hyperlink ref="B12" r:id="rId27" xr:uid="{2C8B3443-48AE-472B-8B71-94EE65EDAD01}"/>
+    <hyperlink ref="B14" r:id="rId28" xr:uid="{304D21BB-CA92-4A54-8547-375084292F85}"/>
+    <hyperlink ref="F12" r:id="rId29" xr:uid="{9008EE1B-E8AE-4A0D-984F-B12DD1DAB45D}"/>
+    <hyperlink ref="F14" r:id="rId30" xr:uid="{573D0817-1969-4B68-A9EA-1A1C9EFBCC06}"/>
+    <hyperlink ref="B38" r:id="rId31" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
+    <hyperlink ref="F38" r:id="rId32" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
     <hyperlink ref="B3" r:id="rId33" xr:uid="{C7795FC0-8B33-4D93-9DFE-3DE6E23A65D1}"/>
     <hyperlink ref="B5" r:id="rId34" xr:uid="{4278CAA6-D3DF-451A-9859-70B12A20B924}"/>
     <hyperlink ref="B7" r:id="rId35" xr:uid="{2FABA182-9872-4794-87EF-110E523D4322}"/>
-    <hyperlink ref="B14" r:id="rId36" xr:uid="{BBA7DCA1-B4D3-4FF3-B86E-BA8861D6C155}"/>
-    <hyperlink ref="B16" r:id="rId37" xr:uid="{70C63C82-C88D-4754-892F-01184B0C7E74}"/>
-    <hyperlink ref="B18" r:id="rId38" xr:uid="{6DF50FF0-316A-44B6-B4C3-FBC9AA28340D}"/>
-    <hyperlink ref="B20" r:id="rId39" xr:uid="{19B2BF48-0496-4713-93FB-06411F9687AF}"/>
-    <hyperlink ref="B23" r:id="rId40" xr:uid="{CEEFBC18-79AB-4B6F-9166-5C92FFF8EE31}"/>
-    <hyperlink ref="B22" r:id="rId41" xr:uid="{9957DDBC-B608-4FC5-82E4-2D3347616AF4}"/>
-    <hyperlink ref="B25" r:id="rId42" xr:uid="{C7CAA40A-FB8B-4C4A-9B0C-E71E249B4EB0}"/>
-    <hyperlink ref="B28" r:id="rId43" xr:uid="{022935CF-4A06-4F9B-9898-B419F332C013}"/>
-    <hyperlink ref="B30" r:id="rId44" xr:uid="{114F977D-6AD3-45F4-AE7E-251DB2F9ED27}"/>
-    <hyperlink ref="B32" r:id="rId45" xr:uid="{C71A1019-DDCB-45D7-B84E-5894071C24F3}"/>
-    <hyperlink ref="B33" r:id="rId46" xr:uid="{200C0C02-6E8B-4A1E-AF6A-EB50D6699F64}"/>
-    <hyperlink ref="B35" r:id="rId47" xr:uid="{0BC1C7ED-E15C-453D-99AE-002352B851F9}"/>
-    <hyperlink ref="B36" r:id="rId48" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
-    <hyperlink ref="B37" r:id="rId49" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
-    <hyperlink ref="B38" r:id="rId50" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
+    <hyperlink ref="B13" r:id="rId36" xr:uid="{BBA7DCA1-B4D3-4FF3-B86E-BA8861D6C155}"/>
+    <hyperlink ref="B15" r:id="rId37" xr:uid="{70C63C82-C88D-4754-892F-01184B0C7E74}"/>
+    <hyperlink ref="B17" r:id="rId38" xr:uid="{6DF50FF0-316A-44B6-B4C3-FBC9AA28340D}"/>
+    <hyperlink ref="B19" r:id="rId39" xr:uid="{19B2BF48-0496-4713-93FB-06411F9687AF}"/>
+    <hyperlink ref="B22" r:id="rId40" xr:uid="{CEEFBC18-79AB-4B6F-9166-5C92FFF8EE31}"/>
+    <hyperlink ref="B21" r:id="rId41" xr:uid="{9957DDBC-B608-4FC5-82E4-2D3347616AF4}"/>
+    <hyperlink ref="B24" r:id="rId42" xr:uid="{C7CAA40A-FB8B-4C4A-9B0C-E71E249B4EB0}"/>
+    <hyperlink ref="B27" r:id="rId43" xr:uid="{022935CF-4A06-4F9B-9898-B419F332C013}"/>
+    <hyperlink ref="B29" r:id="rId44" xr:uid="{114F977D-6AD3-45F4-AE7E-251DB2F9ED27}"/>
+    <hyperlink ref="B31" r:id="rId45" xr:uid="{C71A1019-DDCB-45D7-B84E-5894071C24F3}"/>
+    <hyperlink ref="B32" r:id="rId46" xr:uid="{200C0C02-6E8B-4A1E-AF6A-EB50D6699F64}"/>
+    <hyperlink ref="B34" r:id="rId47" xr:uid="{0BC1C7ED-E15C-453D-99AE-002352B851F9}"/>
+    <hyperlink ref="B35" r:id="rId48" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
+    <hyperlink ref="B36" r:id="rId49" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
+    <hyperlink ref="B37" r:id="rId50" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
     <hyperlink ref="F3" r:id="rId51" xr:uid="{90E44E29-1B03-4447-B24D-9A7BEFA0B242}"/>
     <hyperlink ref="F5" r:id="rId52" xr:uid="{58815120-49BF-4288-8F93-551FA78D11C9}"/>
     <hyperlink ref="F7" r:id="rId53" xr:uid="{F3FFFCCD-EFDC-4AF5-A536-D65140B8A706}"/>
-    <hyperlink ref="F14" r:id="rId54" xr:uid="{3AF944D3-C956-48BD-94DA-DA45F2952A4E}"/>
-    <hyperlink ref="F16" r:id="rId55" xr:uid="{7DCDD4E4-62C1-48AC-AF5A-661760B99205}"/>
-    <hyperlink ref="F18" r:id="rId56" xr:uid="{C42DFCAB-0437-4ED8-A834-2559B815A5A6}"/>
-    <hyperlink ref="F20" r:id="rId57" xr:uid="{E1B17A57-2625-43EB-9E9A-B0C90AA37EC9}"/>
-    <hyperlink ref="F23" r:id="rId58" xr:uid="{5FAE5AE8-C296-4A0A-938C-DEF7DDC99648}"/>
-    <hyperlink ref="F22" r:id="rId59" location="pymorphy2" xr:uid="{72E80F3F-0CDB-413E-9CEF-61AD10CE13DF}"/>
-    <hyperlink ref="F25" r:id="rId60" xr:uid="{F6A0975B-9838-4ED3-AA23-D1E9FFED4559}"/>
-    <hyperlink ref="F28" r:id="rId61" xr:uid="{B83A70D9-0117-4193-BB82-D5C5304E242C}"/>
-    <hyperlink ref="F30" r:id="rId62" xr:uid="{21FD9621-3F04-4514-9C1B-BE58D52EE36A}"/>
-    <hyperlink ref="F32" r:id="rId63" xr:uid="{A97408C0-8C57-4522-B48B-D9DA8A5487C8}"/>
-    <hyperlink ref="F33" r:id="rId64" xr:uid="{8ABCFE54-79FA-41FC-835F-BF3C64A34270}"/>
-    <hyperlink ref="F35" r:id="rId65" xr:uid="{D6220873-36F4-4C46-9C7B-068E9FEE6D5B}"/>
-    <hyperlink ref="F36" r:id="rId66" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
-    <hyperlink ref="F37" r:id="rId67" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
-    <hyperlink ref="F38" r:id="rId68" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
+    <hyperlink ref="F13" r:id="rId54" xr:uid="{3AF944D3-C956-48BD-94DA-DA45F2952A4E}"/>
+    <hyperlink ref="F15" r:id="rId55" xr:uid="{7DCDD4E4-62C1-48AC-AF5A-661760B99205}"/>
+    <hyperlink ref="F17" r:id="rId56" xr:uid="{C42DFCAB-0437-4ED8-A834-2559B815A5A6}"/>
+    <hyperlink ref="F19" r:id="rId57" xr:uid="{E1B17A57-2625-43EB-9E9A-B0C90AA37EC9}"/>
+    <hyperlink ref="F22" r:id="rId58" xr:uid="{5FAE5AE8-C296-4A0A-938C-DEF7DDC99648}"/>
+    <hyperlink ref="F21" r:id="rId59" location="pymorphy2" xr:uid="{72E80F3F-0CDB-413E-9CEF-61AD10CE13DF}"/>
+    <hyperlink ref="F24" r:id="rId60" xr:uid="{F6A0975B-9838-4ED3-AA23-D1E9FFED4559}"/>
+    <hyperlink ref="F27" r:id="rId61" xr:uid="{B83A70D9-0117-4193-BB82-D5C5304E242C}"/>
+    <hyperlink ref="F29" r:id="rId62" xr:uid="{21FD9621-3F04-4514-9C1B-BE58D52EE36A}"/>
+    <hyperlink ref="F31" r:id="rId63" xr:uid="{A97408C0-8C57-4522-B48B-D9DA8A5487C8}"/>
+    <hyperlink ref="F32" r:id="rId64" xr:uid="{8ABCFE54-79FA-41FC-835F-BF3C64A34270}"/>
+    <hyperlink ref="F34" r:id="rId65" xr:uid="{D6220873-36F4-4C46-9C7B-068E9FEE6D5B}"/>
+    <hyperlink ref="F35" r:id="rId66" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
+    <hyperlink ref="F36" r:id="rId67" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
+    <hyperlink ref="F37" r:id="rId68" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
     <hyperlink ref="B6" r:id="rId69" xr:uid="{52BABBB5-CE0D-46C7-BE77-4A172346845A}"/>
-    <hyperlink ref="B10" r:id="rId70" xr:uid="{DF1A3009-4DC5-4898-9E1D-30D33622D910}"/>
-    <hyperlink ref="B11" r:id="rId71" xr:uid="{BF4812D7-1AE4-4E56-A19F-7C9EC8FD9582}"/>
-    <hyperlink ref="B34" r:id="rId72" xr:uid="{015E9C9A-18B2-4374-8C47-218B22BBB453}"/>
-    <hyperlink ref="F6" r:id="rId73" xr:uid="{1CA61469-520E-4077-B3F9-35C9602CCE35}"/>
-    <hyperlink ref="F10" r:id="rId74" xr:uid="{572F9DBA-601D-47F3-A9D2-732785451947}"/>
-    <hyperlink ref="F11" r:id="rId75" xr:uid="{481FC442-3C4D-4E19-AEE8-B1E6341E9093}"/>
-    <hyperlink ref="F34" r:id="rId76" xr:uid="{C49D23ED-4B53-45F7-8717-1BB92879BB78}"/>
+    <hyperlink ref="B10" r:id="rId70" xr:uid="{BF4812D7-1AE4-4E56-A19F-7C9EC8FD9582}"/>
+    <hyperlink ref="B33" r:id="rId71" xr:uid="{015E9C9A-18B2-4374-8C47-218B22BBB453}"/>
+    <hyperlink ref="F6" r:id="rId72" xr:uid="{1CA61469-520E-4077-B3F9-35C9602CCE35}"/>
+    <hyperlink ref="F10" r:id="rId73" xr:uid="{481FC442-3C4D-4E19-AEE8-B1E6341E9093}"/>
+    <hyperlink ref="F33" r:id="rId74" xr:uid="{C49D23ED-4B53-45F7-8717-1BB92879BB78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId75"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Dependencies: Remove syntok; Utils: Remove syntok's sentence segmenter and word tokenizer
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1453F006-BD31-48FE-A839-B3F7266E3CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A473B9-1829-4353-AC16-E793B4594A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="193">
   <si>
     <t>Python</t>
   </si>
@@ -274,21 +274,6 @@
   </si>
   <si>
     <t>https://github.com/ponrawee/ssg/blob/master/LICENSE</t>
-  </si>
-  <si>
-    <t>syntok</t>
-  </si>
-  <si>
-    <t>https://github.com/fnl/syntok</t>
-  </si>
-  <si>
-    <t>1.3.1</t>
-  </si>
-  <si>
-    <t>Florian Leitner</t>
-  </si>
-  <si>
-    <t>https://github.com/fnl/syntok/blob/master/LICENSE</t>
   </si>
   <si>
     <t>TextBlob</t>
@@ -990,13 +975,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C140BD20-F5FB-434E-99AB-C043EB24C86B}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,22 +1017,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1058,7 +1043,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
@@ -1072,22 +1057,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1101,7 +1086,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
@@ -1112,27 +1097,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -1152,102 +1137,102 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1272,22 +1257,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1298,7 +1283,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>42</v>
@@ -1312,22 +1297,22 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,22 +1337,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1381,7 +1366,7 @@
         <v>51</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>14</v>
@@ -1398,7 +1383,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>7</v>
@@ -1467,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1478,10 +1463,10 @@
         <v>65</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>25</v>
@@ -1512,22 +1497,22 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1552,22 +1537,22 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1578,7 +1563,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>74</v>
@@ -1592,22 +1577,22 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1615,13 +1600,13 @@
         <v>76</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>14</v>
@@ -1652,22 +1637,22 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1675,56 +1660,56 @@
         <v>83</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>177</v>
-      </c>
       <c r="C35" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>94</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>95</v>
@@ -1732,47 +1717,27 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>97</v>
+        <v>171</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F38">
-    <sortCondition ref="A2:A38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
+    <sortCondition ref="A2:A37"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CF73D8A8-B4D6-4683-89DA-FFC51092EBEB}"/>
@@ -1805,8 +1770,8 @@
     <hyperlink ref="B14" r:id="rId28" xr:uid="{304D21BB-CA92-4A54-8547-375084292F85}"/>
     <hyperlink ref="F12" r:id="rId29" xr:uid="{9008EE1B-E8AE-4A0D-984F-B12DD1DAB45D}"/>
     <hyperlink ref="F14" r:id="rId30" xr:uid="{573D0817-1969-4B68-A9EA-1A1C9EFBCC06}"/>
-    <hyperlink ref="B38" r:id="rId31" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
-    <hyperlink ref="F38" r:id="rId32" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
+    <hyperlink ref="B37" r:id="rId31" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
+    <hyperlink ref="F37" r:id="rId32" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
     <hyperlink ref="B3" r:id="rId33" xr:uid="{C7795FC0-8B33-4D93-9DFE-3DE6E23A65D1}"/>
     <hyperlink ref="B5" r:id="rId34" xr:uid="{4278CAA6-D3DF-451A-9859-70B12A20B924}"/>
     <hyperlink ref="B7" r:id="rId35" xr:uid="{2FABA182-9872-4794-87EF-110E523D4322}"/>
@@ -1821,37 +1786,35 @@
     <hyperlink ref="B29" r:id="rId44" xr:uid="{114F977D-6AD3-45F4-AE7E-251DB2F9ED27}"/>
     <hyperlink ref="B31" r:id="rId45" xr:uid="{C71A1019-DDCB-45D7-B84E-5894071C24F3}"/>
     <hyperlink ref="B32" r:id="rId46" xr:uid="{200C0C02-6E8B-4A1E-AF6A-EB50D6699F64}"/>
-    <hyperlink ref="B34" r:id="rId47" xr:uid="{0BC1C7ED-E15C-453D-99AE-002352B851F9}"/>
-    <hyperlink ref="B35" r:id="rId48" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
-    <hyperlink ref="B36" r:id="rId49" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
-    <hyperlink ref="B37" r:id="rId50" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
-    <hyperlink ref="F3" r:id="rId51" xr:uid="{90E44E29-1B03-4447-B24D-9A7BEFA0B242}"/>
-    <hyperlink ref="F5" r:id="rId52" xr:uid="{58815120-49BF-4288-8F93-551FA78D11C9}"/>
-    <hyperlink ref="F7" r:id="rId53" xr:uid="{F3FFFCCD-EFDC-4AF5-A536-D65140B8A706}"/>
-    <hyperlink ref="F13" r:id="rId54" xr:uid="{3AF944D3-C956-48BD-94DA-DA45F2952A4E}"/>
-    <hyperlink ref="F15" r:id="rId55" xr:uid="{7DCDD4E4-62C1-48AC-AF5A-661760B99205}"/>
-    <hyperlink ref="F17" r:id="rId56" xr:uid="{C42DFCAB-0437-4ED8-A834-2559B815A5A6}"/>
-    <hyperlink ref="F19" r:id="rId57" xr:uid="{E1B17A57-2625-43EB-9E9A-B0C90AA37EC9}"/>
-    <hyperlink ref="F22" r:id="rId58" xr:uid="{5FAE5AE8-C296-4A0A-938C-DEF7DDC99648}"/>
-    <hyperlink ref="F21" r:id="rId59" location="pymorphy2" xr:uid="{72E80F3F-0CDB-413E-9CEF-61AD10CE13DF}"/>
-    <hyperlink ref="F24" r:id="rId60" xr:uid="{F6A0975B-9838-4ED3-AA23-D1E9FFED4559}"/>
-    <hyperlink ref="F27" r:id="rId61" xr:uid="{B83A70D9-0117-4193-BB82-D5C5304E242C}"/>
-    <hyperlink ref="F29" r:id="rId62" xr:uid="{21FD9621-3F04-4514-9C1B-BE58D52EE36A}"/>
-    <hyperlink ref="F31" r:id="rId63" xr:uid="{A97408C0-8C57-4522-B48B-D9DA8A5487C8}"/>
-    <hyperlink ref="F32" r:id="rId64" xr:uid="{8ABCFE54-79FA-41FC-835F-BF3C64A34270}"/>
-    <hyperlink ref="F34" r:id="rId65" xr:uid="{D6220873-36F4-4C46-9C7B-068E9FEE6D5B}"/>
-    <hyperlink ref="F35" r:id="rId66" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
-    <hyperlink ref="F36" r:id="rId67" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
-    <hyperlink ref="F37" r:id="rId68" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
-    <hyperlink ref="B6" r:id="rId69" xr:uid="{52BABBB5-CE0D-46C7-BE77-4A172346845A}"/>
-    <hyperlink ref="B10" r:id="rId70" xr:uid="{BF4812D7-1AE4-4E56-A19F-7C9EC8FD9582}"/>
-    <hyperlink ref="B33" r:id="rId71" xr:uid="{015E9C9A-18B2-4374-8C47-218B22BBB453}"/>
-    <hyperlink ref="F6" r:id="rId72" xr:uid="{1CA61469-520E-4077-B3F9-35C9602CCE35}"/>
-    <hyperlink ref="F10" r:id="rId73" xr:uid="{481FC442-3C4D-4E19-AEE8-B1E6341E9093}"/>
-    <hyperlink ref="F33" r:id="rId74" xr:uid="{C49D23ED-4B53-45F7-8717-1BB92879BB78}"/>
+    <hyperlink ref="B34" r:id="rId47" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
+    <hyperlink ref="B35" r:id="rId48" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
+    <hyperlink ref="B36" r:id="rId49" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
+    <hyperlink ref="F3" r:id="rId50" xr:uid="{90E44E29-1B03-4447-B24D-9A7BEFA0B242}"/>
+    <hyperlink ref="F5" r:id="rId51" xr:uid="{58815120-49BF-4288-8F93-551FA78D11C9}"/>
+    <hyperlink ref="F7" r:id="rId52" xr:uid="{F3FFFCCD-EFDC-4AF5-A536-D65140B8A706}"/>
+    <hyperlink ref="F13" r:id="rId53" xr:uid="{3AF944D3-C956-48BD-94DA-DA45F2952A4E}"/>
+    <hyperlink ref="F15" r:id="rId54" xr:uid="{7DCDD4E4-62C1-48AC-AF5A-661760B99205}"/>
+    <hyperlink ref="F17" r:id="rId55" xr:uid="{C42DFCAB-0437-4ED8-A834-2559B815A5A6}"/>
+    <hyperlink ref="F19" r:id="rId56" xr:uid="{E1B17A57-2625-43EB-9E9A-B0C90AA37EC9}"/>
+    <hyperlink ref="F22" r:id="rId57" xr:uid="{5FAE5AE8-C296-4A0A-938C-DEF7DDC99648}"/>
+    <hyperlink ref="F21" r:id="rId58" location="pymorphy2" xr:uid="{72E80F3F-0CDB-413E-9CEF-61AD10CE13DF}"/>
+    <hyperlink ref="F24" r:id="rId59" xr:uid="{F6A0975B-9838-4ED3-AA23-D1E9FFED4559}"/>
+    <hyperlink ref="F27" r:id="rId60" xr:uid="{B83A70D9-0117-4193-BB82-D5C5304E242C}"/>
+    <hyperlink ref="F29" r:id="rId61" xr:uid="{21FD9621-3F04-4514-9C1B-BE58D52EE36A}"/>
+    <hyperlink ref="F31" r:id="rId62" xr:uid="{A97408C0-8C57-4522-B48B-D9DA8A5487C8}"/>
+    <hyperlink ref="F32" r:id="rId63" xr:uid="{8ABCFE54-79FA-41FC-835F-BF3C64A34270}"/>
+    <hyperlink ref="F34" r:id="rId64" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
+    <hyperlink ref="F35" r:id="rId65" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
+    <hyperlink ref="F36" r:id="rId66" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
+    <hyperlink ref="B6" r:id="rId67" xr:uid="{52BABBB5-CE0D-46C7-BE77-4A172346845A}"/>
+    <hyperlink ref="B10" r:id="rId68" xr:uid="{BF4812D7-1AE4-4E56-A19F-7C9EC8FD9582}"/>
+    <hyperlink ref="B33" r:id="rId69" xr:uid="{015E9C9A-18B2-4374-8C47-218B22BBB453}"/>
+    <hyperlink ref="F6" r:id="rId70" xr:uid="{1CA61469-520E-4077-B3F9-35C9602CCE35}"/>
+    <hyperlink ref="F10" r:id="rId71" xr:uid="{481FC442-3C4D-4E19-AEE8-B1E6341E9093}"/>
+    <hyperlink ref="F33" r:id="rId72" xr:uid="{C49D23ED-4B53-45F7-8717-1BB92879BB78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId75"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId73"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Doc: Update README - Acknowledgments
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A473B9-1829-4353-AC16-E793B4594A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0D226F-7294-4E3E-A49A-5C29AFCE877E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="188">
   <si>
     <t>Python</t>
   </si>
@@ -454,21 +454,6 @@
   </si>
   <si>
     <t>https://github.com/saffsd/langid.py/blob/master/LICENSE</t>
-  </si>
-  <si>
-    <t>lxml</t>
-  </si>
-  <si>
-    <t>https://lxml.de/</t>
-  </si>
-  <si>
-    <t>4.6.3</t>
-  </si>
-  <si>
-    <t>Stefan Behnel</t>
-  </si>
-  <si>
-    <t>https://github.com/lxml/lxml/blob/master/doc/licenses/BSD.txt</t>
   </si>
   <si>
     <t>NumPy</t>
@@ -975,13 +960,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C140BD20-F5FB-434E-99AB-C043EB24C86B}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1008,7 @@
         <v>125</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>126</v>
@@ -1043,7 +1028,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
@@ -1063,7 +1048,7 @@
         <v>129</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>130</v>
@@ -1086,7 +1071,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
@@ -1117,7 +1102,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -1197,624 +1182,602 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>111</v>
+        <v>35</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>180</v>
+        <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>165</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>170</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>118</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>40</v>
+        <v>143</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>144</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>42</v>
+        <v>145</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>148</v>
+        <v>44</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>182</v>
+        <v>46</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>150</v>
+        <v>47</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>151</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>152</v>
+        <v>49</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>153</v>
+        <v>50</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>154</v>
+        <v>51</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="E19" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>8</v>
+      <c r="F20" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>21</v>
+      <c r="F25" s="8" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>157</v>
+        <v>68</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>158</v>
+        <v>69</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>159</v>
+        <v>70</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>67</v>
+        <v>156</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>68</v>
+        <v>164</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>163</v>
+        <v>74</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="F30" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>178</v>
+        <v>80</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>107</v>
+        <v>167</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>172</v>
+        <v>88</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>84</v>
+        <v>182</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>187</v>
+        <v>93</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="8" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
-    <sortCondition ref="A2:A37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CF73D8A8-B4D6-4683-89DA-FFC51092EBEB}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{771C650C-0717-49FD-B0EC-BF2F40F224EB}"/>
     <hyperlink ref="B8" r:id="rId3" xr:uid="{E12C1CA8-5B68-4852-BA02-BD7BBD2E879E}"/>
     <hyperlink ref="B9" r:id="rId4" xr:uid="{1663737B-16F3-42B6-90CA-BFEB7DCE1174}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{13EDF357-B8BF-4BDF-8117-199BDDBEB4EF}"/>
-    <hyperlink ref="B16" r:id="rId6" xr:uid="{A0E84A41-E233-42F2-BD8A-A1BDF1E81869}"/>
-    <hyperlink ref="B18" r:id="rId7" xr:uid="{4F5A65A0-DA16-4EAA-8204-89C4587728EC}"/>
-    <hyperlink ref="B26" r:id="rId8" xr:uid="{D806A658-6D50-416A-8F31-9519F420DB6F}"/>
-    <hyperlink ref="B28" r:id="rId9" xr:uid="{AE9E7534-DCC6-43F9-9F7E-CB7D0988653C}"/>
-    <hyperlink ref="B30" r:id="rId10" xr:uid="{48E985F1-8312-44D5-B359-BC5428959610}"/>
-    <hyperlink ref="F2" r:id="rId11" xr:uid="{929E88FE-A5CA-4C8A-AB63-CC5216646638}"/>
-    <hyperlink ref="F4" r:id="rId12" xr:uid="{FF1D0CA5-516F-4B32-914F-109BD9394062}"/>
-    <hyperlink ref="F8" r:id="rId13" xr:uid="{56571F8E-94F9-4E59-8301-FD9B586601E2}"/>
-    <hyperlink ref="F9" r:id="rId14" xr:uid="{4E203B3A-56CE-4F2E-8E50-ECD13E173A62}"/>
-    <hyperlink ref="F11" r:id="rId15" xr:uid="{F43F53F1-7279-4683-9981-2134AA1FD339}"/>
-    <hyperlink ref="F16" r:id="rId16" xr:uid="{C85E458B-00C2-411B-B49E-AE8022969698}"/>
-    <hyperlink ref="F18" r:id="rId17" xr:uid="{976B8A16-77B7-4FEF-9169-6BBFE075FCA3}"/>
-    <hyperlink ref="F26" r:id="rId18" xr:uid="{A52538D1-12B7-46FF-8221-0E6B9ABCA510}"/>
-    <hyperlink ref="F28" r:id="rId19" xr:uid="{7E1954E6-38DA-415E-A3C7-E1A13CC34AA6}"/>
-    <hyperlink ref="F30" r:id="rId20" xr:uid="{24AF1213-EF9C-4A65-A07F-FA87ED52B38E}"/>
-    <hyperlink ref="F25" r:id="rId21" location="psf-license-agreement-for-python-release" xr:uid="{F5F51C21-2025-43C8-A97E-01655AD44B0D}"/>
-    <hyperlink ref="F20" r:id="rId22" xr:uid="{5E4BF004-2691-47C7-8862-14F66FADDDD6}"/>
-    <hyperlink ref="F23" r:id="rId23" location="license" xr:uid="{660E8A5C-2DFD-41A4-861A-90E9BF510D8D}"/>
-    <hyperlink ref="B25" r:id="rId24" xr:uid="{D099E31D-9265-415C-969C-6D26EB302243}"/>
-    <hyperlink ref="B20" r:id="rId25" xr:uid="{5AE99205-01DB-477E-A6BD-69F46164974B}"/>
-    <hyperlink ref="B23" r:id="rId26" xr:uid="{0F7B6A32-4F56-4F52-A479-8662313527D4}"/>
-    <hyperlink ref="B12" r:id="rId27" xr:uid="{2C8B3443-48AE-472B-8B71-94EE65EDAD01}"/>
-    <hyperlink ref="B14" r:id="rId28" xr:uid="{304D21BB-CA92-4A54-8547-375084292F85}"/>
-    <hyperlink ref="F12" r:id="rId29" xr:uid="{9008EE1B-E8AE-4A0D-984F-B12DD1DAB45D}"/>
-    <hyperlink ref="F14" r:id="rId30" xr:uid="{573D0817-1969-4B68-A9EA-1A1C9EFBCC06}"/>
-    <hyperlink ref="B37" r:id="rId31" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
-    <hyperlink ref="F37" r:id="rId32" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
-    <hyperlink ref="B3" r:id="rId33" xr:uid="{C7795FC0-8B33-4D93-9DFE-3DE6E23A65D1}"/>
-    <hyperlink ref="B5" r:id="rId34" xr:uid="{4278CAA6-D3DF-451A-9859-70B12A20B924}"/>
-    <hyperlink ref="B7" r:id="rId35" xr:uid="{2FABA182-9872-4794-87EF-110E523D4322}"/>
-    <hyperlink ref="B13" r:id="rId36" xr:uid="{BBA7DCA1-B4D3-4FF3-B86E-BA8861D6C155}"/>
-    <hyperlink ref="B15" r:id="rId37" xr:uid="{70C63C82-C88D-4754-892F-01184B0C7E74}"/>
-    <hyperlink ref="B17" r:id="rId38" xr:uid="{6DF50FF0-316A-44B6-B4C3-FBC9AA28340D}"/>
-    <hyperlink ref="B19" r:id="rId39" xr:uid="{19B2BF48-0496-4713-93FB-06411F9687AF}"/>
-    <hyperlink ref="B22" r:id="rId40" xr:uid="{CEEFBC18-79AB-4B6F-9166-5C92FFF8EE31}"/>
-    <hyperlink ref="B21" r:id="rId41" xr:uid="{9957DDBC-B608-4FC5-82E4-2D3347616AF4}"/>
-    <hyperlink ref="B24" r:id="rId42" xr:uid="{C7CAA40A-FB8B-4C4A-9B0C-E71E249B4EB0}"/>
-    <hyperlink ref="B27" r:id="rId43" xr:uid="{022935CF-4A06-4F9B-9898-B419F332C013}"/>
-    <hyperlink ref="B29" r:id="rId44" xr:uid="{114F977D-6AD3-45F4-AE7E-251DB2F9ED27}"/>
-    <hyperlink ref="B31" r:id="rId45" xr:uid="{C71A1019-DDCB-45D7-B84E-5894071C24F3}"/>
-    <hyperlink ref="B32" r:id="rId46" xr:uid="{200C0C02-6E8B-4A1E-AF6A-EB50D6699F64}"/>
-    <hyperlink ref="B34" r:id="rId47" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
-    <hyperlink ref="B35" r:id="rId48" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
-    <hyperlink ref="B36" r:id="rId49" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
-    <hyperlink ref="F3" r:id="rId50" xr:uid="{90E44E29-1B03-4447-B24D-9A7BEFA0B242}"/>
-    <hyperlink ref="F5" r:id="rId51" xr:uid="{58815120-49BF-4288-8F93-551FA78D11C9}"/>
-    <hyperlink ref="F7" r:id="rId52" xr:uid="{F3FFFCCD-EFDC-4AF5-A536-D65140B8A706}"/>
-    <hyperlink ref="F13" r:id="rId53" xr:uid="{3AF944D3-C956-48BD-94DA-DA45F2952A4E}"/>
-    <hyperlink ref="F15" r:id="rId54" xr:uid="{7DCDD4E4-62C1-48AC-AF5A-661760B99205}"/>
-    <hyperlink ref="F17" r:id="rId55" xr:uid="{C42DFCAB-0437-4ED8-A834-2559B815A5A6}"/>
-    <hyperlink ref="F19" r:id="rId56" xr:uid="{E1B17A57-2625-43EB-9E9A-B0C90AA37EC9}"/>
-    <hyperlink ref="F22" r:id="rId57" xr:uid="{5FAE5AE8-C296-4A0A-938C-DEF7DDC99648}"/>
-    <hyperlink ref="F21" r:id="rId58" location="pymorphy2" xr:uid="{72E80F3F-0CDB-413E-9CEF-61AD10CE13DF}"/>
-    <hyperlink ref="F24" r:id="rId59" xr:uid="{F6A0975B-9838-4ED3-AA23-D1E9FFED4559}"/>
-    <hyperlink ref="F27" r:id="rId60" xr:uid="{B83A70D9-0117-4193-BB82-D5C5304E242C}"/>
-    <hyperlink ref="F29" r:id="rId61" xr:uid="{21FD9621-3F04-4514-9C1B-BE58D52EE36A}"/>
-    <hyperlink ref="F31" r:id="rId62" xr:uid="{A97408C0-8C57-4522-B48B-D9DA8A5487C8}"/>
-    <hyperlink ref="F32" r:id="rId63" xr:uid="{8ABCFE54-79FA-41FC-835F-BF3C64A34270}"/>
-    <hyperlink ref="F34" r:id="rId64" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
-    <hyperlink ref="F35" r:id="rId65" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
-    <hyperlink ref="F36" r:id="rId66" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
-    <hyperlink ref="B6" r:id="rId67" xr:uid="{52BABBB5-CE0D-46C7-BE77-4A172346845A}"/>
-    <hyperlink ref="B10" r:id="rId68" xr:uid="{BF4812D7-1AE4-4E56-A19F-7C9EC8FD9582}"/>
-    <hyperlink ref="B33" r:id="rId69" xr:uid="{015E9C9A-18B2-4374-8C47-218B22BBB453}"/>
-    <hyperlink ref="F6" r:id="rId70" xr:uid="{1CA61469-520E-4077-B3F9-35C9602CCE35}"/>
-    <hyperlink ref="F10" r:id="rId71" xr:uid="{481FC442-3C4D-4E19-AEE8-B1E6341E9093}"/>
-    <hyperlink ref="F33" r:id="rId72" xr:uid="{C49D23ED-4B53-45F7-8717-1BB92879BB78}"/>
+    <hyperlink ref="B15" r:id="rId5" xr:uid="{A0E84A41-E233-42F2-BD8A-A1BDF1E81869}"/>
+    <hyperlink ref="B17" r:id="rId6" xr:uid="{4F5A65A0-DA16-4EAA-8204-89C4587728EC}"/>
+    <hyperlink ref="B25" r:id="rId7" xr:uid="{D806A658-6D50-416A-8F31-9519F420DB6F}"/>
+    <hyperlink ref="B27" r:id="rId8" xr:uid="{AE9E7534-DCC6-43F9-9F7E-CB7D0988653C}"/>
+    <hyperlink ref="B29" r:id="rId9" xr:uid="{48E985F1-8312-44D5-B359-BC5428959610}"/>
+    <hyperlink ref="F2" r:id="rId10" xr:uid="{929E88FE-A5CA-4C8A-AB63-CC5216646638}"/>
+    <hyperlink ref="F4" r:id="rId11" xr:uid="{FF1D0CA5-516F-4B32-914F-109BD9394062}"/>
+    <hyperlink ref="F8" r:id="rId12" xr:uid="{56571F8E-94F9-4E59-8301-FD9B586601E2}"/>
+    <hyperlink ref="F9" r:id="rId13" xr:uid="{4E203B3A-56CE-4F2E-8E50-ECD13E173A62}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{C85E458B-00C2-411B-B49E-AE8022969698}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{976B8A16-77B7-4FEF-9169-6BBFE075FCA3}"/>
+    <hyperlink ref="F25" r:id="rId16" xr:uid="{A52538D1-12B7-46FF-8221-0E6B9ABCA510}"/>
+    <hyperlink ref="F27" r:id="rId17" xr:uid="{7E1954E6-38DA-415E-A3C7-E1A13CC34AA6}"/>
+    <hyperlink ref="F29" r:id="rId18" xr:uid="{24AF1213-EF9C-4A65-A07F-FA87ED52B38E}"/>
+    <hyperlink ref="F24" r:id="rId19" location="psf-license-agreement-for-python-release" xr:uid="{F5F51C21-2025-43C8-A97E-01655AD44B0D}"/>
+    <hyperlink ref="F19" r:id="rId20" xr:uid="{5E4BF004-2691-47C7-8862-14F66FADDDD6}"/>
+    <hyperlink ref="F22" r:id="rId21" location="license" xr:uid="{660E8A5C-2DFD-41A4-861A-90E9BF510D8D}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{D099E31D-9265-415C-969C-6D26EB302243}"/>
+    <hyperlink ref="B19" r:id="rId23" xr:uid="{5AE99205-01DB-477E-A6BD-69F46164974B}"/>
+    <hyperlink ref="B22" r:id="rId24" xr:uid="{0F7B6A32-4F56-4F52-A479-8662313527D4}"/>
+    <hyperlink ref="B11" r:id="rId25" xr:uid="{2C8B3443-48AE-472B-8B71-94EE65EDAD01}"/>
+    <hyperlink ref="B13" r:id="rId26" xr:uid="{304D21BB-CA92-4A54-8547-375084292F85}"/>
+    <hyperlink ref="F11" r:id="rId27" xr:uid="{9008EE1B-E8AE-4A0D-984F-B12DD1DAB45D}"/>
+    <hyperlink ref="F13" r:id="rId28" xr:uid="{573D0817-1969-4B68-A9EA-1A1C9EFBCC06}"/>
+    <hyperlink ref="B36" r:id="rId29" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
+    <hyperlink ref="F36" r:id="rId30" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
+    <hyperlink ref="B3" r:id="rId31" xr:uid="{C7795FC0-8B33-4D93-9DFE-3DE6E23A65D1}"/>
+    <hyperlink ref="B5" r:id="rId32" xr:uid="{4278CAA6-D3DF-451A-9859-70B12A20B924}"/>
+    <hyperlink ref="B7" r:id="rId33" xr:uid="{2FABA182-9872-4794-87EF-110E523D4322}"/>
+    <hyperlink ref="B12" r:id="rId34" xr:uid="{BBA7DCA1-B4D3-4FF3-B86E-BA8861D6C155}"/>
+    <hyperlink ref="B14" r:id="rId35" xr:uid="{70C63C82-C88D-4754-892F-01184B0C7E74}"/>
+    <hyperlink ref="B16" r:id="rId36" xr:uid="{6DF50FF0-316A-44B6-B4C3-FBC9AA28340D}"/>
+    <hyperlink ref="B18" r:id="rId37" xr:uid="{19B2BF48-0496-4713-93FB-06411F9687AF}"/>
+    <hyperlink ref="B21" r:id="rId38" xr:uid="{CEEFBC18-79AB-4B6F-9166-5C92FFF8EE31}"/>
+    <hyperlink ref="B20" r:id="rId39" xr:uid="{9957DDBC-B608-4FC5-82E4-2D3347616AF4}"/>
+    <hyperlink ref="B23" r:id="rId40" xr:uid="{C7CAA40A-FB8B-4C4A-9B0C-E71E249B4EB0}"/>
+    <hyperlink ref="B26" r:id="rId41" xr:uid="{022935CF-4A06-4F9B-9898-B419F332C013}"/>
+    <hyperlink ref="B28" r:id="rId42" xr:uid="{114F977D-6AD3-45F4-AE7E-251DB2F9ED27}"/>
+    <hyperlink ref="B30" r:id="rId43" xr:uid="{C71A1019-DDCB-45D7-B84E-5894071C24F3}"/>
+    <hyperlink ref="B31" r:id="rId44" xr:uid="{200C0C02-6E8B-4A1E-AF6A-EB50D6699F64}"/>
+    <hyperlink ref="B33" r:id="rId45" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
+    <hyperlink ref="B34" r:id="rId46" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
+    <hyperlink ref="B35" r:id="rId47" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
+    <hyperlink ref="F3" r:id="rId48" xr:uid="{90E44E29-1B03-4447-B24D-9A7BEFA0B242}"/>
+    <hyperlink ref="F5" r:id="rId49" xr:uid="{58815120-49BF-4288-8F93-551FA78D11C9}"/>
+    <hyperlink ref="F7" r:id="rId50" xr:uid="{F3FFFCCD-EFDC-4AF5-A536-D65140B8A706}"/>
+    <hyperlink ref="F12" r:id="rId51" xr:uid="{3AF944D3-C956-48BD-94DA-DA45F2952A4E}"/>
+    <hyperlink ref="F14" r:id="rId52" xr:uid="{7DCDD4E4-62C1-48AC-AF5A-661760B99205}"/>
+    <hyperlink ref="F16" r:id="rId53" xr:uid="{C42DFCAB-0437-4ED8-A834-2559B815A5A6}"/>
+    <hyperlink ref="F18" r:id="rId54" xr:uid="{E1B17A57-2625-43EB-9E9A-B0C90AA37EC9}"/>
+    <hyperlink ref="F21" r:id="rId55" xr:uid="{5FAE5AE8-C296-4A0A-938C-DEF7DDC99648}"/>
+    <hyperlink ref="F20" r:id="rId56" location="pymorphy2" xr:uid="{72E80F3F-0CDB-413E-9CEF-61AD10CE13DF}"/>
+    <hyperlink ref="F23" r:id="rId57" xr:uid="{F6A0975B-9838-4ED3-AA23-D1E9FFED4559}"/>
+    <hyperlink ref="F26" r:id="rId58" xr:uid="{B83A70D9-0117-4193-BB82-D5C5304E242C}"/>
+    <hyperlink ref="F28" r:id="rId59" xr:uid="{21FD9621-3F04-4514-9C1B-BE58D52EE36A}"/>
+    <hyperlink ref="F30" r:id="rId60" xr:uid="{A97408C0-8C57-4522-B48B-D9DA8A5487C8}"/>
+    <hyperlink ref="F31" r:id="rId61" xr:uid="{8ABCFE54-79FA-41FC-835F-BF3C64A34270}"/>
+    <hyperlink ref="F33" r:id="rId62" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
+    <hyperlink ref="F34" r:id="rId63" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
+    <hyperlink ref="F35" r:id="rId64" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
+    <hyperlink ref="B6" r:id="rId65" xr:uid="{52BABBB5-CE0D-46C7-BE77-4A172346845A}"/>
+    <hyperlink ref="B10" r:id="rId66" xr:uid="{BF4812D7-1AE4-4E56-A19F-7C9EC8FD9582}"/>
+    <hyperlink ref="B32" r:id="rId67" xr:uid="{015E9C9A-18B2-4374-8C47-218B22BBB453}"/>
+    <hyperlink ref="F6" r:id="rId68" xr:uid="{1CA61469-520E-4077-B3F9-35C9602CCE35}"/>
+    <hyperlink ref="F10" r:id="rId69" xr:uid="{481FC442-3C4D-4E19-AEE8-B1E6341E9093}"/>
+    <hyperlink ref="F32" r:id="rId70" xr:uid="{C49D23ED-4B53-45F7-8717-1BB92879BB78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId73"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId71"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Dependencies: Upgrade Pyphen to 0.12.0
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0D226F-7294-4E3E-A49A-5C29AFCE877E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5CCEC2-418F-42EA-B5B1-3A8F094E7B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,9 +192,6 @@
     <t>https://pyphen.org/</t>
   </si>
   <si>
-    <t>0.11.0</t>
-  </si>
-  <si>
     <t>Guillaume Ayoub</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>3.2.1</t>
+  </si>
+  <si>
+    <t>0.12.0</t>
   </si>
 </sst>
 </file>
@@ -963,10 +963,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,22 +1002,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1028,7 +1028,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>24</v>
@@ -1042,22 +1042,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1071,7 +1071,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>14</v>
@@ -1082,27 +1082,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>31</v>
@@ -1122,82 +1122,82 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>135</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1222,22 +1222,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1248,7 +1248,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>42</v>
@@ -1262,22 +1262,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1302,22 +1302,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1331,7 +1331,7 @@
         <v>51</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>14</v>
@@ -1348,7 +1348,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
@@ -1362,22 +1362,22 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1388,16 +1388,16 @@
         <v>54</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1417,27 +1417,27 @@
         <v>13</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="C23" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1462,242 +1462,242 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependencies: Upgrade PyQt to 5.15.6
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5CCEC2-418F-42EA-B5B1-3A8F094E7B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307754ED-2EB0-4088-A5F1-994C7A7EA422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>https://riverbankcomputing.com/software/pyqt/</t>
   </si>
   <si>
-    <t>5.15.4</t>
-  </si>
-  <si>
     <t>Riverbank Computing Limited</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>0.12.0</t>
+  </si>
+  <si>
+    <t>5.15.6</t>
   </si>
 </sst>
 </file>
@@ -963,10 +963,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,362 +982,362 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>116</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1348,7 +1348,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
@@ -1362,42 +1362,42 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1408,36 +1408,36 @@
         <v>10</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="F22" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1457,247 +1457,247 @@
         <v>4</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="E26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="E28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="E32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D34" s="7" t="s">
+      <c r="E34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D36" s="7" t="s">
+      <c r="E36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependencies: Upgrade TextBlob to 0.17.1
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307754ED-2EB0-4088-A5F1-994C7A7EA422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB63E76-0535-4331-A4FA-F5B716E847DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>TextBlob</t>
   </si>
   <si>
-    <t>0.15.3</t>
-  </si>
-  <si>
     <t>Steven Loria</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>5.15.6</t>
+  </si>
+  <si>
+    <t>0.17.1</t>
   </si>
 </sst>
 </file>
@@ -963,10 +963,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,22 +1002,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1028,7 +1028,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1042,22 +1042,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1071,7 +1071,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>13</v>
@@ -1082,27 +1082,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>30</v>
@@ -1122,82 +1122,82 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1222,22 +1222,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1248,7 +1248,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>41</v>
@@ -1262,22 +1262,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1302,22 +1302,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1331,7 +1331,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>13</v>
@@ -1348,7 +1348,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
@@ -1388,7 +1388,7 @@
         <v>53</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>54</v>
@@ -1408,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>11</v>
@@ -1417,7 +1417,7 @@
         <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1428,10 +1428,10 @@
         <v>63</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
@@ -1462,22 +1462,22 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1502,22 +1502,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1528,7 +1528,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>72</v>
@@ -1542,22 +1542,22 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1565,13 +1565,13 @@
         <v>74</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>13</v>
@@ -1602,22 +1602,22 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1625,79 +1625,79 @@
         <v>81</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependencies: Upgrade NLTK to 3.6.7
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB63E76-0535-4331-A4FA-F5B716E847DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA367FF-9CD4-47F1-B6D8-43A095F43E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,9 +576,6 @@
     <t>0.8.8</t>
   </si>
   <si>
-    <t>3.6.5</t>
-  </si>
-  <si>
     <t>2.0.9</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
   </si>
   <si>
     <t>0.17.1</t>
+  </si>
+  <si>
+    <t>3.6.7</t>
   </si>
 </sst>
 </file>
@@ -963,10 +963,10 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +1048,7 @@
         <v>126</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>127</v>
@@ -1248,7 +1248,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>41</v>
@@ -1388,7 +1388,7 @@
         <v>53</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>54</v>
@@ -1408,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>11</v>
@@ -1568,7 +1568,7 @@
         <v>120</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>170</v>
@@ -1628,7 +1628,7 @@
         <v>164</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Dependencies: Add SudachiPy; Utils: Add SudachiPy's Japanese word tokenizer, POS tagger, and lemmatizer
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA367FF-9CD4-47F1-B6D8-43A095F43E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECEBF9E-F651-4C97-976D-49377436DDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="193">
   <si>
     <t>Python</t>
   </si>
@@ -592,6 +592,21 @@
   </si>
   <si>
     <t>3.6.7</t>
+  </si>
+  <si>
+    <t>SudachiPy</t>
+  </si>
+  <si>
+    <t>0.6.2</t>
+  </si>
+  <si>
+    <t>https://github.com/WorksApplications/sudachi.rs</t>
+  </si>
+  <si>
+    <t>Works Applications Co., Ltd.</t>
+  </si>
+  <si>
+    <t>https://github.com/WorksApplications/sudachi.rs/blob/develop/LICENSE</t>
   </si>
 </sst>
 </file>
@@ -960,13 +975,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C140BD20-F5FB-434E-99AB-C043EB24C86B}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1622,87 +1637,107 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>82</v>
+        <v>191</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>83</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>90</v>
+        <v>179</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D37" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F36">
-    <sortCondition ref="A2:A36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
+    <sortCondition ref="A2:A37"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CF73D8A8-B4D6-4683-89DA-FFC51092EBEB}"/>
@@ -1733,8 +1768,8 @@
     <hyperlink ref="B13" r:id="rId26" xr:uid="{304D21BB-CA92-4A54-8547-375084292F85}"/>
     <hyperlink ref="F11" r:id="rId27" xr:uid="{9008EE1B-E8AE-4A0D-984F-B12DD1DAB45D}"/>
     <hyperlink ref="F13" r:id="rId28" xr:uid="{573D0817-1969-4B68-A9EA-1A1C9EFBCC06}"/>
-    <hyperlink ref="B36" r:id="rId29" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
-    <hyperlink ref="F36" r:id="rId30" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
+    <hyperlink ref="B37" r:id="rId29" xr:uid="{1D8B4B2E-07BC-441B-8045-C6DA2F3E44CF}"/>
+    <hyperlink ref="F37" r:id="rId30" xr:uid="{5BA45FDA-3287-48BB-9116-C244765FD800}"/>
     <hyperlink ref="B3" r:id="rId31" xr:uid="{C7795FC0-8B33-4D93-9DFE-3DE6E23A65D1}"/>
     <hyperlink ref="B5" r:id="rId32" xr:uid="{4278CAA6-D3DF-451A-9859-70B12A20B924}"/>
     <hyperlink ref="B7" r:id="rId33" xr:uid="{2FABA182-9872-4794-87EF-110E523D4322}"/>
@@ -1749,9 +1784,9 @@
     <hyperlink ref="B28" r:id="rId42" xr:uid="{114F977D-6AD3-45F4-AE7E-251DB2F9ED27}"/>
     <hyperlink ref="B30" r:id="rId43" xr:uid="{C71A1019-DDCB-45D7-B84E-5894071C24F3}"/>
     <hyperlink ref="B31" r:id="rId44" xr:uid="{200C0C02-6E8B-4A1E-AF6A-EB50D6699F64}"/>
-    <hyperlink ref="B33" r:id="rId45" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
-    <hyperlink ref="B34" r:id="rId46" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
-    <hyperlink ref="B35" r:id="rId47" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
+    <hyperlink ref="B34" r:id="rId45" xr:uid="{234EEB35-509B-4726-A637-669325880B47}"/>
+    <hyperlink ref="B35" r:id="rId46" xr:uid="{AFA18DE8-D7D3-4C9F-8978-6542797E2A10}"/>
+    <hyperlink ref="B36" r:id="rId47" xr:uid="{B5165E08-9C47-4F72-B38A-110FDE1F4EC8}"/>
     <hyperlink ref="F3" r:id="rId48" xr:uid="{90E44E29-1B03-4447-B24D-9A7BEFA0B242}"/>
     <hyperlink ref="F5" r:id="rId49" xr:uid="{58815120-49BF-4288-8F93-551FA78D11C9}"/>
     <hyperlink ref="F7" r:id="rId50" xr:uid="{F3FFFCCD-EFDC-4AF5-A536-D65140B8A706}"/>
@@ -1766,9 +1801,9 @@
     <hyperlink ref="F28" r:id="rId59" xr:uid="{21FD9621-3F04-4514-9C1B-BE58D52EE36A}"/>
     <hyperlink ref="F30" r:id="rId60" xr:uid="{A97408C0-8C57-4522-B48B-D9DA8A5487C8}"/>
     <hyperlink ref="F31" r:id="rId61" xr:uid="{8ABCFE54-79FA-41FC-835F-BF3C64A34270}"/>
-    <hyperlink ref="F33" r:id="rId62" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
-    <hyperlink ref="F34" r:id="rId63" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
-    <hyperlink ref="F35" r:id="rId64" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
+    <hyperlink ref="F34" r:id="rId62" xr:uid="{8F136783-1F04-438D-AF1B-872D35C96EBF}"/>
+    <hyperlink ref="F35" r:id="rId63" xr:uid="{4AB762DC-C549-4DFD-A3FF-AD31F9421E21}"/>
+    <hyperlink ref="F36" r:id="rId64" xr:uid="{69E6CA6E-1F1E-4E70-8FFA-3EEDFDC63D0B}"/>
     <hyperlink ref="B6" r:id="rId65" xr:uid="{52BABBB5-CE0D-46C7-BE77-4A172346845A}"/>
     <hyperlink ref="B10" r:id="rId66" xr:uid="{BF4812D7-1AE4-4E56-A19F-7C9EC8FD9582}"/>
     <hyperlink ref="B32" r:id="rId67" xr:uid="{015E9C9A-18B2-4374-8C47-218B22BBB453}"/>

</xml_diff>

<commit_message>
Dependencies: Upgrade Underthesea to 1.3.4
</commit_message>
<xml_diff>
--- a/src/wl_acks.xlsx
+++ b/src/wl_acks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wordless\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECEBF9E-F651-4C97-976D-49377436DDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E43D11-1A7F-4485-8082-6B2DB0879F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,9 +297,6 @@
     <t>https://github.com/undertheseanlp/underthesea</t>
   </si>
   <si>
-    <t>1.2.2</t>
-  </si>
-  <si>
     <t>Vu Anh</t>
   </si>
   <si>
@@ -607,6 +604,9 @@
   </si>
   <si>
     <t>https://github.com/WorksApplications/sudachi.rs/blob/develop/LICENSE</t>
+  </si>
+  <si>
+    <t>1.3.4</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,22 +1017,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1043,7 +1043,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>23</v>
@@ -1057,22 +1057,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1086,7 +1086,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>13</v>
@@ -1097,27 +1097,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>30</v>
@@ -1137,82 +1137,82 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,22 +1237,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1263,7 +1263,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>41</v>
@@ -1277,22 +1277,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1317,22 +1317,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1346,7 +1346,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>13</v>
@@ -1363,7 +1363,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>7</v>
@@ -1403,7 +1403,7 @@
         <v>53</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>54</v>
@@ -1423,7 +1423,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>11</v>
@@ -1432,7 +1432,7 @@
         <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1443,10 +1443,10 @@
         <v>63</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>24</v>
@@ -1477,22 +1477,22 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>151</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1517,22 +1517,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>155</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1543,7 +1543,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>72</v>
@@ -1557,22 +1557,22 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1580,13 +1580,13 @@
         <v>74</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>13</v>
@@ -1617,42 +1617,42 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>191</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1660,10 +1660,10 @@
         <v>81</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>82</v>
@@ -1683,7 +1683,7 @@
         <v>85</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>86</v>
@@ -1703,36 +1703,36 @@
         <v>89</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>